<commit_message>
db relationships and sql join.
</commit_message>
<xml_diff>
--- a/Info For DB.xlsx
+++ b/Info For DB.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/17eebd954901a7d8/Desktop/Prisoner Of War Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amypa\OneDrive\Desktop\Prisoner Of War Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="81" documentId="8_{B753BC70-A03E-4F4F-9429-AADEFDBF3CE0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{128AA48F-DD5D-4D1E-8168-7A76AF6FDEC7}"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="8_{B753BC70-A03E-4F4F-9429-AADEFDBF3CE0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{E078ED38-7D0B-426F-A81F-1165C448DAFC}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{EF279B8D-0823-43A0-B466-378A44D0F605}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{EF279B8D-0823-43A0-B466-378A44D0F605}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="355">
   <si>
     <t>Pte</t>
   </si>
@@ -761,6 +762,342 @@
   </si>
   <si>
     <t>YMCA 2NZEF</t>
+  </si>
+  <si>
+    <t>Crete</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>13.12.41</t>
+  </si>
+  <si>
+    <t>2.1.42</t>
+  </si>
+  <si>
+    <t>30.11.41</t>
+  </si>
+  <si>
+    <t>8.12.43</t>
+  </si>
+  <si>
+    <t>22.7.42</t>
+  </si>
+  <si>
+    <t>25.1.42</t>
+  </si>
+  <si>
+    <t>1.2.41</t>
+  </si>
+  <si>
+    <t>15.7.42</t>
+  </si>
+  <si>
+    <t>14.7.42</t>
+  </si>
+  <si>
+    <t>28.6.42</t>
+  </si>
+  <si>
+    <t>21.7.42</t>
+  </si>
+  <si>
+    <t>3.9.42</t>
+  </si>
+  <si>
+    <t>13.2.41</t>
+  </si>
+  <si>
+    <t>3.12.43</t>
+  </si>
+  <si>
+    <t>18.2.44</t>
+  </si>
+  <si>
+    <t>21.3.44</t>
+  </si>
+  <si>
+    <t>28.11.43</t>
+  </si>
+  <si>
+    <t>24.12.43</t>
+  </si>
+  <si>
+    <t>25.10.42</t>
+  </si>
+  <si>
+    <t>14.4.43</t>
+  </si>
+  <si>
+    <t>15.12.42</t>
+  </si>
+  <si>
+    <t>19.3.44</t>
+  </si>
+  <si>
+    <t>16.7.42</t>
+  </si>
+  <si>
+    <t>21.1.42</t>
+  </si>
+  <si>
+    <t>22.1.42</t>
+  </si>
+  <si>
+    <t>17.3.44</t>
+  </si>
+  <si>
+    <t>24.7.42</t>
+  </si>
+  <si>
+    <t>28.11.41</t>
+  </si>
+  <si>
+    <t>4.9.42</t>
+  </si>
+  <si>
+    <t>18.12.41</t>
+  </si>
+  <si>
+    <t>22.11.41</t>
+  </si>
+  <si>
+    <t>20.4.43</t>
+  </si>
+  <si>
+    <t>16.12.42</t>
+  </si>
+  <si>
+    <t>4.7.42</t>
+  </si>
+  <si>
+    <t>25.10.43</t>
+  </si>
+  <si>
+    <t>22.6.42</t>
+  </si>
+  <si>
+    <t>1.12.41</t>
+  </si>
+  <si>
+    <t>12.2.41</t>
+  </si>
+  <si>
+    <t>28.8.42</t>
+  </si>
+  <si>
+    <t>16.12.43</t>
+  </si>
+  <si>
+    <t>26.11.41</t>
+  </si>
+  <si>
+    <t>19.7.42</t>
+  </si>
+  <si>
+    <t>7.12.43</t>
+  </si>
+  <si>
+    <t>27.6.42</t>
+  </si>
+  <si>
+    <t>23.10.42</t>
+  </si>
+  <si>
+    <t>9.2.44</t>
+  </si>
+  <si>
+    <t>22.12.42</t>
+  </si>
+  <si>
+    <t>2.12.41</t>
+  </si>
+  <si>
+    <t>1.7.42</t>
+  </si>
+  <si>
+    <t>20.2.44</t>
+  </si>
+  <si>
+    <t>29.6.42</t>
+  </si>
+  <si>
+    <t>15.7.43</t>
+  </si>
+  <si>
+    <t>26.6.42</t>
+  </si>
+  <si>
+    <t>7.2.44</t>
+  </si>
+  <si>
+    <t>11.12.43</t>
+  </si>
+  <si>
+    <t>3.12.42</t>
+  </si>
+  <si>
+    <t>17.7.42</t>
+  </si>
+  <si>
+    <t>28.12.42</t>
+  </si>
+  <si>
+    <t>2.11.42</t>
+  </si>
+  <si>
+    <t>30.8.42</t>
+  </si>
+  <si>
+    <t>28.11.42</t>
+  </si>
+  <si>
+    <t>7.7.42</t>
+  </si>
+  <si>
+    <t>23.11.41</t>
+  </si>
+  <si>
+    <t>27.7.42</t>
+  </si>
+  <si>
+    <t>30.3.44</t>
+  </si>
+  <si>
+    <t>11.7.42</t>
+  </si>
+  <si>
+    <t>14.9.42</t>
+  </si>
+  <si>
+    <t>26.4.43</t>
+  </si>
+  <si>
+    <t>5.7.42</t>
+  </si>
+  <si>
+    <t>26.8.42</t>
+  </si>
+  <si>
+    <t>25.5.42</t>
+  </si>
+  <si>
+    <t>2.12.43</t>
+  </si>
+  <si>
+    <t>3.7.42</t>
+  </si>
+  <si>
+    <t>5.11.42</t>
+  </si>
+  <si>
+    <t>23.7.42</t>
+  </si>
+  <si>
+    <t>29.5.44</t>
+  </si>
+  <si>
+    <t>Greece/Crete</t>
+  </si>
+  <si>
+    <t>16.3.44</t>
+  </si>
+  <si>
+    <t>6.7.42</t>
+  </si>
+  <si>
+    <t>2.6.42</t>
+  </si>
+  <si>
+    <t>13.12.42</t>
+  </si>
+  <si>
+    <t>5.6.43</t>
+  </si>
+  <si>
+    <t>10.8.42</t>
+  </si>
+  <si>
+    <t>3.4.43</t>
+  </si>
+  <si>
+    <t>3.12.41</t>
+  </si>
+  <si>
+    <t>22.9.42</t>
+  </si>
+  <si>
+    <t>20.6.42</t>
+  </si>
+  <si>
+    <t>26.3.43</t>
+  </si>
+  <si>
+    <t>28.5.44</t>
+  </si>
+  <si>
+    <t>3.2.43</t>
+  </si>
+  <si>
+    <t>9.7.42</t>
+  </si>
+  <si>
+    <t>27.10.42</t>
+  </si>
+  <si>
+    <t>13.11.41</t>
+  </si>
+  <si>
+    <t>?.7.42</t>
+  </si>
+  <si>
+    <t>7.11.42</t>
+  </si>
+  <si>
+    <t>9.10.42</t>
+  </si>
+  <si>
+    <t>1.8.44</t>
+  </si>
+  <si>
+    <t>21.11.43</t>
+  </si>
+  <si>
+    <t>16.1.43</t>
+  </si>
+  <si>
+    <t>15.11.43</t>
+  </si>
+  <si>
+    <t>28.7.44</t>
+  </si>
+  <si>
+    <t>?.?.42</t>
+  </si>
+  <si>
+    <t>20.11.41</t>
+  </si>
+  <si>
+    <t>22.11.43</t>
+  </si>
+  <si>
+    <t>Battle Of Crete</t>
+  </si>
+  <si>
+    <t>Battle Of Greece</t>
+  </si>
+  <si>
+    <t>Battle of Jitra (British Empire)</t>
+  </si>
+  <si>
+    <t>Battle of Kampar (United Kingdom)</t>
+  </si>
+  <si>
+    <t>Japan Troops Sieze Control of Manila, Philipines</t>
+  </si>
+  <si>
+    <t>Operation Crusader</t>
   </si>
 </sst>
 </file>
@@ -1592,7 +1929,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD7EF18A-4E88-4B41-BA28-4913ECD20240}">
   <dimension ref="A1:B138"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2298,4 +2635,576 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C9D3AA5-3598-4B1C-AD61-BCE77EB71202}">
+  <dimension ref="A1:C106"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="35.5546875" customWidth="1"/>
+    <col min="3" max="3" width="39.44140625" customWidth="1"/>
+    <col min="4" max="4" width="35.44140625" customWidth="1"/>
+    <col min="5" max="5" width="26.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B2" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B3" t="s">
+        <v>351</v>
+      </c>
+      <c r="C3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>246</v>
+      </c>
+      <c r="B4" t="s">
+        <v>352</v>
+      </c>
+      <c r="C4" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>247</v>
+      </c>
+      <c r="B5" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>348</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
rewrote the prisoner information template, with styling.
</commit_message>
<xml_diff>
--- a/Info For DB.xlsx
+++ b/Info For DB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amypa\OneDrive\Desktop\Prisoner Of War Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="8_{B753BC70-A03E-4F4F-9429-AADEFDBF3CE0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{E078ED38-7D0B-426F-A81F-1165C448DAFC}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="8_{B753BC70-A03E-4F4F-9429-AADEFDBF3CE0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{E743EA7D-16D7-4F87-8FD4-012DF522022D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{EF279B8D-0823-43A0-B466-378A44D0F605}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{EF279B8D-0823-43A0-B466-378A44D0F605}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="357">
   <si>
     <t>Pte</t>
   </si>
@@ -1098,6 +1098,12 @@
   </si>
   <si>
     <t>Operation Crusader</t>
+  </si>
+  <si>
+    <t>Purpose of Role</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is the lowest rank within the miltary. </t>
   </si>
 </sst>
 </file>
@@ -1452,34 +1458,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B85E5437-3A3D-4714-B916-E74A8F6D5B20}">
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="3" max="3" width="53.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>59</v>
       </c>
       <c r="B1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1487,7 +1500,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1495,7 +1508,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1503,7 +1516,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1511,7 +1524,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1519,7 +1532,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1527,7 +1540,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1535,7 +1548,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1543,7 +1556,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1551,7 +1564,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1559,7 +1572,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1567,7 +1580,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1575,7 +1588,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1583,7 +1596,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -2641,7 +2654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C9D3AA5-3598-4B1C-AD61-BCE77EB71202}">
   <dimension ref="A1:C106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>